<commit_message>
Small changes to performance profile plots.
</commit_message>
<xml_diff>
--- a/code/results/storm_j10_7200/compact_reformulation_trans_results_j10.xlsx
+++ b/code/results/storm_j10_7200/compact_reformulation_trans_results_j10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="compact_reformulation_trans_results_0" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="554">
   <si>
     <t xml:space="preserve">instance</t>
   </si>
@@ -1666,6 +1666,9 @@
     <t xml:space="preserve">avg. solve time</t>
   </si>
   <si>
+    <t xml:space="preserve">(incl. 7200 for instances not solved to optimality)</t>
+  </si>
+  <si>
     <t xml:space="preserve">avg avg solve time</t>
   </si>
   <si>
@@ -1679,6 +1682,9 @@
   </si>
   <si>
     <t xml:space="preserve">avg. opt objval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg. opt objval (solved for all Gamma)</t>
   </si>
 </sst>
 </file>
@@ -1779,10 +1785,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L537"/>
+  <dimension ref="A1:O537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F520" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M553" activeCellId="0" sqref="M553"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A496" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K537" activeCellId="0" sqref="K537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12422,10 +12428,10 @@
         <f aca="false">100*COUNTIF(E2:E537,0)/ROWS(E2:E537)</f>
         <v>100</v>
       </c>
-      <c r="K531" s="0" t="s">
+      <c r="N531" s="0" t="s">
         <v>537</v>
       </c>
-      <c r="L531" s="0" t="n">
+      <c r="O531" s="0" t="n">
         <f aca="false">AVERAGE(compact_reformulation_trans_results_0:compact_reformulation_trans_results_7!I531:I531)</f>
         <v>100</v>
       </c>
@@ -12483,10 +12489,10 @@
         <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
         <v>0</v>
       </c>
-      <c r="K533" s="0" t="s">
+      <c r="N533" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="L533" s="0" t="n">
+      <c r="O533" s="0" t="n">
         <f aca="false">AVERAGE(compact_reformulation_trans_results_0:compact_reformulation_trans_results_7!I533:I533)</f>
         <v>0</v>
       </c>
@@ -12544,17 +12550,20 @@
         <f aca="false">AVERAGE(F2:F537)</f>
         <v>1.83836567164179</v>
       </c>
-      <c r="K535" s="0" t="s">
+      <c r="J535" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="L535" s="0" t="n">
+      <c r="N535" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="O535" s="0" t="n">
         <f aca="false">AVERAGE(compact_reformulation_trans_results_0:compact_reformulation_trans_results_7!I535:I535)</f>
         <v>4.47083815298508</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>0</v>
@@ -12572,7 +12581,7 @@
         <v>0.125</v>
       </c>
       <c r="H536" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I536" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;7200")</f>
@@ -12581,7 +12590,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>0</v>
@@ -12599,10 +12608,17 @@
         <v>0.059</v>
       </c>
       <c r="H537" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I537" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"=0",C2:C537)</f>
+        <v>16.8432835820896</v>
+      </c>
+      <c r="K537" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="L537" s="0" t="n">
+        <f aca="false">AVERAGEIFS(C2:C537, compact_reformulation_trans_results_0!E2:E537, "=0",compact_reformulation_trans_results_3!E2:E537, "=0", compact_reformulation_trans_results_5!E2:E537, "=0", compact_reformulation_trans_results_7!E2:E537, "=0")</f>
         <v>16.8432835820896</v>
       </c>
     </row>
@@ -12622,10 +12638,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I537"/>
+  <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A519" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H531" activeCellId="0" sqref="H531"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A527" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23373,10 +23389,13 @@
         <f aca="false">AVERAGE(F2:F537)</f>
         <v>4.96213432835821</v>
       </c>
+      <c r="J535" s="1" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>3</v>
@@ -23394,7 +23413,7 @@
         <v>0.33</v>
       </c>
       <c r="H536" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I536" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;7200")</f>
@@ -23403,7 +23422,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>3</v>
@@ -23421,10 +23440,17 @@
         <v>0.439</v>
       </c>
       <c r="H537" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I537" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"=0",C2:C537)</f>
+        <v>25.3414179104478</v>
+      </c>
+      <c r="K537" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="L537" s="0" t="n">
+        <f aca="false">AVERAGEIFS(C2:C537, compact_reformulation_trans_results_0!E2:E537, "=0",compact_reformulation_trans_results_3!E2:E537, "=0", compact_reformulation_trans_results_5!E2:E537, "=0", compact_reformulation_trans_results_7!E2:E537, "=0")</f>
         <v>25.3414179104478</v>
       </c>
     </row>
@@ -23444,10 +23470,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I537"/>
+  <dimension ref="A1:L537"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A507" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H531" activeCellId="0" sqref="H531"/>
+      <selection pane="topLeft" activeCell="K537" activeCellId="0" sqref="K537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34195,10 +34221,13 @@
         <f aca="false">AVERAGE(F2:F537)</f>
         <v>4.61833768656717</v>
       </c>
+      <c r="J535" s="1" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>5</v>
@@ -34216,7 +34245,7 @@
         <v>0.681</v>
       </c>
       <c r="H536" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I536" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;7200")</f>
@@ -34225,7 +34254,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>5</v>
@@ -34243,10 +34272,17 @@
         <v>1.464</v>
       </c>
       <c r="H537" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I537" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"=0",C2:C537)</f>
+        <v>26.3526119402985</v>
+      </c>
+      <c r="K537" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="L537" s="0" t="n">
+        <f aca="false">AVERAGEIFS(C2:C537, compact_reformulation_trans_results_0!E2:E537, "=0",compact_reformulation_trans_results_3!E2:E537, "=0", compact_reformulation_trans_results_5!E2:E537, "=0", compact_reformulation_trans_results_7!E2:E537, "=0")</f>
         <v>26.3526119402985</v>
       </c>
     </row>
@@ -34266,10 +34302,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I537"/>
+  <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A521" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I531" activeCellId="0" sqref="I531"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A521" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45017,10 +45053,13 @@
         <f aca="false">AVERAGE(F2:F537)</f>
         <v>6.46451492537314</v>
       </c>
+      <c r="J535" s="1" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>7</v>
@@ -45038,7 +45077,7 @@
         <v>0.546</v>
       </c>
       <c r="H536" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I536" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;7200")</f>
@@ -45047,7 +45086,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>7</v>
@@ -45065,10 +45104,17 @@
         <v>0.408</v>
       </c>
       <c r="H537" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="I537" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"=0",C2:C537)</f>
+        <v>26.4626865671642</v>
+      </c>
+      <c r="K537" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="L537" s="0" t="n">
+        <f aca="false">AVERAGEIFS(C2:C537, compact_reformulation_trans_results_0!E2:E537, "=0",compact_reformulation_trans_results_3!E2:E537, "=0", compact_reformulation_trans_results_5!E2:E537, "=0", compact_reformulation_trans_results_7!E2:E537, "=0")</f>
         <v>26.4626865671642</v>
       </c>
     </row>

</xml_diff>